<commit_message>
Added Dring CNC Modules
</commit_message>
<xml_diff>
--- a/Hardware/Main Board V1.2/Connection_Notes.xlsx
+++ b/Hardware/Main Board V1.2/Connection_Notes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\Plasma-Board\Hardware\Main Board V1.2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52F756B2-E8F4-4869-B932-9C72F1121D7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BA6A677-5470-44AD-80BC-FBEFDA4D9933}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="2" xr2:uid="{3758BE0A-FED1-4CE6-972E-E965A802D2E7}"/>
+    <workbookView xWindow="41865" yWindow="5025" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{3758BE0A-FED1-4CE6-972E-E965A802D2E7}"/>
   </bookViews>
   <sheets>
     <sheet name="Connectors" sheetId="2" r:id="rId1"/>
@@ -29,6 +29,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">Connectors!$P$4:$Z$66</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>

</xml_diff>